<commit_message>
Überarbeitete Dialogskizzen und Dialogbeschreibungen
</commit_message>
<xml_diff>
--- a/Dokumente/02_Arbeitsbereich/04_Anforderungsspezifikation/Dialogbeschreibungen/Spiel_Laden_Fenster_Beschreibung.xlsx
+++ b/Dokumente/02_Arbeitsbereich/04_Anforderungsspezifikation/Dialogbeschreibungen/Spiel_Laden_Fenster_Beschreibung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANTJOOLLI\Desktop\SE_Projekt2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66E2A80E-DBC1-4730-9FC4-3E26E8EB5FF4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21137DF4-FBE0-4C9D-BE45-948AE94BFAE7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="0" windowWidth="20520" windowHeight="10635" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -69,10 +69,25 @@
     <t>Datei Auswählen</t>
   </si>
   <si>
-    <t>Es wird ein Explorer Fenster geöffnet um eine Speicherdatei zum laden auszuwählen.</t>
-  </si>
-  <si>
     <t>Lädt das Spiel, erstellt die Lobby und gibt diese zum Login für Spieler der geladenen Partie frei. Wechselt dann zum Dialogfenster Host(Pregame)</t>
+  </si>
+  <si>
+    <t>Ausgewählte Datei</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Name der ausgewählten Datei</t>
+  </si>
+  <si>
+    <t>Benötigte Mitspieler</t>
+  </si>
+  <si>
+    <t>Namen der Benötigten Mitspieler</t>
+  </si>
+  <si>
+    <t>Es wird ein Explorer Fenster geöffnet um eine Speicherdatei zum laden auszuwählen. Nach dem auswählen wird das Label benötigte Mitspieler aus dieser Datei befüllt</t>
   </si>
 </sst>
 </file>
@@ -449,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F9" sqref="F8:F9"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -515,7 +530,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -524,7 +539,7 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
@@ -536,19 +551,31 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+    <row r="8" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>